<commit_message>
atualização dos dados do gráfico
</commit_message>
<xml_diff>
--- a/Grafico SO.xlsx
+++ b/Grafico SO.xlsx
@@ -119,35 +119,35 @@
           </c:val>
         </c:ser>
         <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>400 x 400</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>154.19999999999999</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:val>
+        </c:ser>
+        <c:ser>
           <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:v>300 x 300</c:v>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numLit>
-              <c:formatCode>General</c:formatCode>
-              <c:ptCount val="1"/>
-              <c:pt idx="0">
-                <c:v>64.2</c:v>
-              </c:pt>
-            </c:numLit>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
           <c:order val="3"/>
           <c:tx>
-            <c:v>400 x 400</c:v>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numLit>
-              <c:formatCode>General</c:formatCode>
-              <c:ptCount val="1"/>
-              <c:pt idx="0">
-                <c:v>154.19999999999999</c:v>
+            <c:v>800 x 800</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>1730.5</c:v>
               </c:pt>
             </c:numLit>
           </c:val>
@@ -156,15 +156,15 @@
           <c:idx val="4"/>
           <c:order val="4"/>
           <c:tx>
-            <c:v>500 x 500</c:v>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numLit>
-              <c:formatCode>General</c:formatCode>
-              <c:ptCount val="1"/>
-              <c:pt idx="0">
-                <c:v>301.89999999999998</c:v>
+            <c:v>1600 x 1600</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>15888.6</c:v>
               </c:pt>
             </c:numLit>
           </c:val>
@@ -173,32 +173,15 @@
           <c:idx val="5"/>
           <c:order val="5"/>
           <c:tx>
-            <c:v>1000 x 1000</c:v>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numLit>
-              <c:formatCode>General</c:formatCode>
-              <c:ptCount val="1"/>
-              <c:pt idx="0">
-                <c:v>3207.2</c:v>
-              </c:pt>
-            </c:numLit>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="6"/>
-          <c:order val="6"/>
-          <c:tx>
-            <c:v>2000 x 2000</c:v>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numLit>
-              <c:formatCode>General</c:formatCode>
-              <c:ptCount val="1"/>
-              <c:pt idx="0">
-                <c:v>32885.9</c:v>
+            <c:v>3200 x 3200</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>176724.7</c:v>
               </c:pt>
             </c:numLit>
           </c:val>
@@ -212,11 +195,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="200721152"/>
-        <c:axId val="200722688"/>
+        <c:axId val="205181696"/>
+        <c:axId val="205183232"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="200721152"/>
+        <c:axId val="205181696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -225,7 +208,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="200722688"/>
+        <c:crossAx val="205183232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -233,10 +216,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="200722688"/>
+        <c:axId val="205183232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="33000"/>
+          <c:max val="180000"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -246,7 +229,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="200721152"/>
+        <c:crossAx val="205181696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -300,52 +283,52 @@
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="6"/>
+          <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>2000 x 2000 / 32</c:v>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numLit>
-              <c:formatCode>General</c:formatCode>
-              <c:ptCount val="1"/>
-              <c:pt idx="0">
-                <c:v>6258.8</c:v>
-              </c:pt>
-            </c:numLit>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="0"/>
+            <c:v>100 x 100/8</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>1.6</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>2000 x 2000 / 24</c:v>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numLit>
-              <c:formatCode>General</c:formatCode>
-              <c:ptCount val="1"/>
-              <c:pt idx="0">
-                <c:v>5782.9</c:v>
-              </c:pt>
-            </c:numLit>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
+            <c:v>200 x 200/8</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>7.2</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>2000 x 2000 / 16</c:v>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numLit>
-              <c:formatCode>General</c:formatCode>
-              <c:ptCount val="1"/>
-              <c:pt idx="0">
-                <c:v>5786.6</c:v>
+            <c:v>400 x 400/8</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>45.1</c:v>
               </c:pt>
             </c:numLit>
           </c:val>
@@ -354,66 +337,49 @@
           <c:idx val="2"/>
           <c:order val="3"/>
           <c:tx>
-            <c:v>2000 x 2000 / 8</c:v>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numLit>
-              <c:formatCode>General</c:formatCode>
-              <c:ptCount val="1"/>
-              <c:pt idx="0">
-                <c:v>5777.8</c:v>
-              </c:pt>
-            </c:numLit>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
+            <c:v>800 x 800/8</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>338.7</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
           <c:order val="4"/>
           <c:tx>
-            <c:v>2000 x 2000 / 6</c:v>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numLit>
-              <c:formatCode>General</c:formatCode>
-              <c:ptCount val="1"/>
-              <c:pt idx="0">
-                <c:v>5410.5</c:v>
-              </c:pt>
-            </c:numLit>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
+            <c:v>1600 x 1600/8</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>3302.4</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
           <c:order val="5"/>
           <c:tx>
-            <c:v>2000 x 2000 / 4</c:v>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numLit>
-              <c:formatCode>General</c:formatCode>
-              <c:ptCount val="1"/>
-              <c:pt idx="0">
-                <c:v>7318.2</c:v>
-              </c:pt>
-            </c:numLit>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="6"/>
-          <c:tx>
-            <c:v>2000 x 2000 / 2</c:v>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numLit>
-              <c:formatCode>General</c:formatCode>
-              <c:ptCount val="1"/>
-              <c:pt idx="0">
-                <c:v>13767.3</c:v>
+            <c:v>3200 x 3200/8</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>60446.8</c:v>
               </c:pt>
             </c:numLit>
           </c:val>
@@ -427,11 +393,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="201026176"/>
-        <c:axId val="201032064"/>
+        <c:axId val="133277568"/>
+        <c:axId val="133279104"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="201026176"/>
+        <c:axId val="133277568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -440,7 +406,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="201032064"/>
+        <c:crossAx val="133279104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -448,10 +414,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="201032064"/>
+        <c:axId val="133279104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="14000"/>
+          <c:max val="65000"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -461,7 +427,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="201026176"/>
+        <c:crossAx val="133277568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -515,52 +481,52 @@
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="6"/>
+          <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>2000 x 2000 / 32</c:v>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numLit>
-              <c:formatCode>General</c:formatCode>
-              <c:ptCount val="1"/>
-              <c:pt idx="0">
-                <c:v>5926.1</c:v>
-              </c:pt>
-            </c:numLit>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="0"/>
+            <c:v>100 x 100/8</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>1.2</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>2000 x 2000 / 24</c:v>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numLit>
-              <c:formatCode>General</c:formatCode>
-              <c:ptCount val="1"/>
-              <c:pt idx="0">
-                <c:v>5982.5</c:v>
-              </c:pt>
-            </c:numLit>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
+            <c:v>200 x 200/8</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>6.4</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>2000 x 2000 / 16</c:v>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numLit>
-              <c:formatCode>General</c:formatCode>
-              <c:ptCount val="1"/>
-              <c:pt idx="0">
-                <c:v>6105.7</c:v>
+            <c:v>400 x 400/8</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>47.5</c:v>
               </c:pt>
             </c:numLit>
           </c:val>
@@ -569,66 +535,49 @@
           <c:idx val="2"/>
           <c:order val="3"/>
           <c:tx>
-            <c:v>2000 x 2000 / 8</c:v>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numLit>
-              <c:formatCode>General</c:formatCode>
-              <c:ptCount val="1"/>
-              <c:pt idx="0">
-                <c:v>5805.7</c:v>
-              </c:pt>
-            </c:numLit>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
+            <c:v>800 x 800/8</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>396.1</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
           <c:order val="4"/>
           <c:tx>
-            <c:v>2000 x 2000 / 6</c:v>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numLit>
-              <c:formatCode>General</c:formatCode>
-              <c:ptCount val="1"/>
-              <c:pt idx="0">
-                <c:v>5401.8</c:v>
-              </c:pt>
-            </c:numLit>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
+            <c:v>1600 x 1600/8</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>5879.4</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
           <c:order val="5"/>
           <c:tx>
-            <c:v>2000 x 2000 / 4</c:v>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numLit>
-              <c:formatCode>General</c:formatCode>
-              <c:ptCount val="1"/>
-              <c:pt idx="0">
-                <c:v>7467.9</c:v>
-              </c:pt>
-            </c:numLit>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="6"/>
-          <c:tx>
-            <c:v>2000 x 2000 / 2</c:v>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numLit>
-              <c:formatCode>General</c:formatCode>
-              <c:ptCount val="1"/>
-              <c:pt idx="0">
-                <c:v>14262.8</c:v>
+            <c:v>3200 x 3200/8</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>56128</c:v>
               </c:pt>
             </c:numLit>
           </c:val>
@@ -642,11 +591,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="36223616"/>
-        <c:axId val="36229504"/>
+        <c:axId val="140483200"/>
+        <c:axId val="140501376"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="36223616"/>
+        <c:axId val="140483200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -655,7 +604,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="36229504"/>
+        <c:crossAx val="140501376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -663,10 +612,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="36229504"/>
+        <c:axId val="140501376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="15000"/>
+          <c:max val="65000"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -676,7 +625,437 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="36223616"/>
+        <c:crossAx val="140483200"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:solidFill>
+        <a:schemeClr val="tx2">
+          <a:lumMod val="75000"/>
+          <a:alpha val="0"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>3200 x 3200/2</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>94036.1</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>3200 x 3200/4</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>64721.3</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>3200 x 3200/6</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>60438.1</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>3200 x 3200/8</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>60446.8</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>3200 x 3200/16</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>61367.5</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>3200 x 3200/24</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>61151</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:v>3200 x 3200/32</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>60205.5</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="39576320"/>
+        <c:axId val="39577856"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="39576320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="39577856"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="39577856"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="75000"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="39576320"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:solidFill>
+        <a:schemeClr val="tx2">
+          <a:lumMod val="75000"/>
+          <a:alpha val="0"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>3200 x 3200/2</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>135380.5</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>3200 x 3200/4</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>68030.100000000006</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>3200 x 3200/6</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>57756.6</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>3200 x 3200/8</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>56128</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>3200 x 3200/16</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>50387.3</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>3200 x 3200/24</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>48300.3</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:v>3200 x 3200/32</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>47123.7</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="140699904"/>
+        <c:axId val="159711232"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="140699904"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="159711232"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="159711232"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="135000"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="140699904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -713,15 +1092,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:colOff>359020</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>62523</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>34193</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>119672</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -743,19 +1122,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>206375</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:colOff>427403</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>35</xdr:col>
-      <xdr:colOff>492125</xdr:colOff>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>102577</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>120650</xdr:rowOff>
+      <xdr:rowOff>20515</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Gráfico 3" title="Matriz processo"/>
+        <xdr:cNvPr id="6" name="Gráfico 5" title="Processo"/>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -774,20 +1153,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>444500</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>280147</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>127000</xdr:colOff>
-      <xdr:row>62</xdr:row>
-      <xdr:rowOff>136525</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>571644</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>29854</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Gráfico 4" title="Matriz threads"/>
+        <xdr:cNvPr id="7" name="Gráfico 6" title="Thread"/>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -799,6 +1178,70 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>575468</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>119063</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>251809</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>148915</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Gráfico 7" title="Processos Experimento 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>490682</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>57728</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>167022</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>87581</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Gráfico 8" title="Threads Experimento 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1094,10 +1537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T23"/>
+  <dimension ref="A1:T29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="AJ47" sqref="AJ47"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
+      <selection activeCell="V72" sqref="V72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1608,6 +2051,7 @@
       <c r="S23" s="1"/>
       <c r="T23" s="1"/>
     </row>
+    <row r="29" spans="1:20" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
coreção das escalas dos gráficos
</commit_message>
<xml_diff>
--- a/Grafico SO.xlsx
+++ b/Grafico SO.xlsx
@@ -195,11 +195,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="212717568"/>
-        <c:axId val="212719104"/>
+        <c:axId val="215339008"/>
+        <c:axId val="215340544"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="212717568"/>
+        <c:axId val="215339008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -208,7 +208,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="212719104"/>
+        <c:crossAx val="215340544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -216,7 +216,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="212719104"/>
+        <c:axId val="215340544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="180000"/>
@@ -229,7 +229,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="212717568"/>
+        <c:crossAx val="215339008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -393,11 +393,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="213410944"/>
-        <c:axId val="213412480"/>
+        <c:axId val="216028288"/>
+        <c:axId val="216029824"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="213410944"/>
+        <c:axId val="216028288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -406,7 +406,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="213412480"/>
+        <c:crossAx val="216029824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -414,7 +414,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="213412480"/>
+        <c:axId val="216029824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="65000"/>
@@ -427,7 +427,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="213410944"/>
+        <c:crossAx val="216028288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -591,11 +591,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="213457152"/>
-        <c:axId val="213463040"/>
+        <c:axId val="216070400"/>
+        <c:axId val="216076288"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="213457152"/>
+        <c:axId val="216070400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -604,7 +604,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="213463040"/>
+        <c:crossAx val="216076288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -612,7 +612,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="213463040"/>
+        <c:axId val="216076288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="65000"/>
@@ -625,7 +625,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="213457152"/>
+        <c:crossAx val="216070400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -806,11 +806,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="213504384"/>
-        <c:axId val="213505920"/>
+        <c:axId val="216125824"/>
+        <c:axId val="216127360"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="213504384"/>
+        <c:axId val="216125824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -819,7 +819,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="213505920"/>
+        <c:crossAx val="216127360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -827,10 +827,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="213505920"/>
+        <c:axId val="216127360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="75000"/>
+          <c:max val="100000"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -840,7 +840,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="213504384"/>
+        <c:crossAx val="216125824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1021,11 +1021,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="213854464"/>
-        <c:axId val="213864448"/>
+        <c:axId val="216480000"/>
+        <c:axId val="216489984"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="213854464"/>
+        <c:axId val="216480000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1034,7 +1034,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="213864448"/>
+        <c:crossAx val="216489984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1042,10 +1042,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="213864448"/>
+        <c:axId val="216489984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="95000"/>
+          <c:max val="100000"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1055,7 +1055,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="213854464"/>
+        <c:crossAx val="216480000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1539,7 +1539,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
       <selection activeCell="V72" sqref="V72"/>
     </sheetView>
   </sheetViews>

</xml_diff>